<commit_message>
Updated input files for 58-bus network case studies. Changed contents of lib folder. Fixed a bug in UCGUI_solar.m.
</commit_message>
<xml_diff>
--- a/input_files/UC_case_study_58bus_network_A.xlsx
+++ b/input_files/UC_case_study_58bus_network_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bus index" sheetId="5" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Brown coal LV</t>
   </si>
   <si>
-    <t>Sienna</t>
-  </si>
-  <si>
     <t>Brown coal NSA</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t>Utility PV CAN</t>
   </si>
   <si>
-    <t>Orange</t>
-  </si>
-  <si>
     <t>OrangeRed</t>
   </si>
   <si>
@@ -430,6 +424,12 @@
   </si>
   <si>
     <t>Rooftop PV SA</t>
+  </si>
+  <si>
+    <t>Maroon</t>
+  </si>
+  <si>
+    <t>Tomato</t>
   </si>
 </sst>
 </file>
@@ -2493,7 +2493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
@@ -2518,7 +2518,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>34</v>
@@ -2530,10 +2530,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2547,10 +2547,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3">
         <v>101</v>
@@ -2571,10 +2571,10 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" s="3">
         <v>102</v>
@@ -2595,10 +2595,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="3">
         <v>201</v>
@@ -2616,10 +2616,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="3">
         <v>202</v>
@@ -2637,10 +2637,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" s="3">
         <v>203</v>
@@ -2658,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="3">
         <v>204</v>
@@ -2679,7 +2679,7 @@
         <v>1.609</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>29</v>
@@ -2703,10 +2703,10 @@
         <v>1.345</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" s="3">
         <v>206</v>
@@ -2727,7 +2727,7 @@
         <v>32.953000000000003</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>29</v>
@@ -2751,10 +2751,10 @@
         <v>1.179</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="3">
         <v>208</v>
@@ -2775,10 +2775,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="3">
         <v>209</v>
@@ -2796,10 +2796,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="3">
         <v>210</v>
@@ -2817,10 +2817,10 @@
         <v>24.69</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="3">
         <v>211</v>
@@ -2841,10 +2841,10 @@
         <v>16.22</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="3">
         <v>212</v>
@@ -2868,7 +2868,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="3">
         <v>213</v>
@@ -2889,7 +2889,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="3">
         <v>214</v>
@@ -2907,10 +2907,10 @@
         <v>0.90500000000000003</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="3">
         <v>215</v>
@@ -2931,10 +2931,10 @@
         <v>10.66</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="3">
         <v>216</v>
@@ -2955,10 +2955,10 @@
         <v>10.323</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="3">
         <v>217</v>
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>30</v>
@@ -3006,7 +3006,7 @@
         <v>26</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="3">
         <v>302</v>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>30</v>
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>30</v>
@@ -3066,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="3">
         <v>305</v>
@@ -3087,10 +3087,10 @@
         <v>37.71</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" s="3">
         <v>306</v>
@@ -3111,10 +3111,10 @@
         <v>8.85</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F27" s="3">
         <v>307</v>
@@ -3135,10 +3135,10 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3">
         <v>308</v>
@@ -3159,7 +3159,7 @@
         <v>3.79</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>30</v>
@@ -3183,10 +3183,10 @@
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="3">
         <v>311</v>
@@ -3207,7 +3207,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="3">
         <v>312</v>
@@ -3231,7 +3231,7 @@
         <v>26</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F32" s="3">
         <v>313</v>
@@ -3252,10 +3252,10 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="3">
         <v>314</v>
@@ -3276,10 +3276,10 @@
         <v>0</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F34" s="3">
         <v>315</v>
@@ -3297,10 +3297,10 @@
         <v>0</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F35" s="3">
         <v>401</v>
@@ -3324,7 +3324,7 @@
         <v>27</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F36" s="3">
         <v>402</v>
@@ -3345,7 +3345,7 @@
         <v>27</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37" s="3">
         <v>403</v>
@@ -3366,7 +3366,7 @@
         <v>27</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" s="3">
         <v>404</v>
@@ -3387,7 +3387,7 @@
         <v>27</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F39" s="3">
         <v>405</v>
@@ -3411,7 +3411,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F40" s="3">
         <v>406</v>
@@ -3435,7 +3435,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" s="3">
         <v>407</v>
@@ -3459,7 +3459,7 @@
         <v>27</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F42" s="3">
         <v>408</v>
@@ -3480,10 +3480,10 @@
         <v>5.78</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F43" s="3">
         <v>409</v>
@@ -3504,10 +3504,10 @@
         <v>5.77</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" s="3">
         <v>410</v>
@@ -3528,10 +3528,10 @@
         <v>33.979999999999997</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" s="3">
         <v>411</v>
@@ -3552,10 +3552,10 @@
         <v>16.75</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F46" s="3">
         <v>412</v>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>31</v>
@@ -3597,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>31</v>
@@ -3618,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>31</v>
@@ -3639,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>31</v>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>32</v>
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>32</v>
@@ -3750,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>32</v>
@@ -3771,7 +3771,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>32</v>
@@ -3819,7 +3819,7 @@
         <v>28</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F58" s="3">
         <v>508</v>
@@ -3840,10 +3840,10 @@
         <v>9.9529999999999994</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F59" s="3">
         <v>509</v>
@@ -3868,7 +3868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3899,19 +3899,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -3932,7 +3932,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3974,7 +3974,7 @@
         <v>0.81699999999999995</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4016,7 +4016,7 @@
         <v>0.76</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4058,7 +4058,7 @@
         <v>0.437</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -6735,7 +6735,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6756,13 +6756,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -6779,10 +6779,10 @@
         <v>0.2555</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -6799,10 +6799,10 @@
         <v>0.21110000000000001</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -6819,10 +6819,10 @@
         <v>0.36980000000000002</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
@@ -6839,10 +6839,10 @@
         <v>0.1636</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
@@ -6850,12 +6850,12 @@
     </row>
     <row r="6" spans="1:6">
       <c r="F6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="F7" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -6874,7 +6874,7 @@
   <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B16" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6913,55 +6913,55 @@
         <v>10</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="O1" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6969,7 +6969,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="6">
         <v>21</v>
@@ -7028,10 +7028,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6">
         <v>50</v>
@@ -7090,10 +7090,10 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C4" s="6">
         <v>35</v>
@@ -7152,10 +7152,10 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="6">
         <v>3</v>
@@ -7214,10 +7214,10 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="C6" s="6">
         <v>4</v>
@@ -7276,10 +7276,10 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="C7" s="6">
         <v>37</v>
@@ -7342,10 +7342,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C8" s="6">
         <v>52</v>
@@ -7404,10 +7404,10 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="C9" s="6">
         <v>5</v>
@@ -7470,10 +7470,10 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="C10" s="6">
         <v>24</v>
@@ -7535,10 +7535,10 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="C11" s="6">
         <v>20</v>
@@ -7597,10 +7597,10 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="C12" s="6">
         <v>34</v>
@@ -7659,10 +7659,10 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="C13" s="6">
         <v>51</v>
@@ -7721,10 +7721,10 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="C14" s="6">
         <v>6</v>
@@ -7783,10 +7783,10 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C15" s="6">
         <v>58</v>
@@ -7845,10 +7845,10 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C16" s="6">
         <v>42</v>
@@ -7907,10 +7907,10 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="C17" s="6">
         <v>14</v>

</xml_diff>